<commit_message>
Revert "InitMesh 호출 방식을 바꿈"
This reverts commit c755d86428abf13e9c4f644b641e275806db70a8.
</commit_message>
<xml_diff>
--- a/Data/PlayerData.xlsx
+++ b/Data/PlayerData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GItData\Space Scavenger\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AB097-7F2B-40A8-B9A9-84D08EBA0B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D83F12-966F-4736-B97D-5AF8ADF39B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="1245" windowWidth="22005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6450" yWindow="2040" windowWidth="22005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Created by LibXL trial version 4.0.4. Please buy the LibXL full version for removing this message.</t>
   </si>
@@ -62,10 +62,6 @@
   </si>
   <si>
     <t>Uranium</t>
-  </si>
-  <si>
-    <t>Mineral</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -453,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IV11"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -727,7 +723,7 @@
     <row r="2" spans="1:256">
       <c r="A2">
         <f>COUNTA(C6:C22)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:256">
@@ -743,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:256">
@@ -751,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:256">
@@ -759,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:256">
@@ -767,7 +763,7 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:256">
@@ -775,15 +771,7 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:256">
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>